<commit_message>
updated formula to take note of blank cells
</commit_message>
<xml_diff>
--- a/widget_measurement_converter.xlsx
+++ b/widget_measurement_converter.xlsx
@@ -114,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,13 +140,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,11 +166,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -469,13 +482,13 @@
   <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="73.7109375" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
@@ -540,9 +553,9 @@
       <c r="F7" s="3">
         <v>126</v>
       </c>
-      <c r="G7" s="4" t="str">
-        <f>CONCATENATE("new Vector4(", ROUND(C7/$C$2,$C$4), "f, ", ROUND(D7/$C$3,$C$4), "f, ", ROUND(F7/$C$3,$C$4), "f, ", ROUND(E7/$C$2,$C$4), "f)")</f>
-        <v>new Vector4(0.02853f, 0.04743f, 0.24901f, 0.94423f)</v>
+      <c r="G7" s="5" t="str">
+        <f>IF(COUNTBLANK(B7:F7)&gt;0,"",CONCATENATE(B7,".Bounds = new Vector4(", ROUND(C7/$C$2,$C$4), "f, ", ROUND(D7/$C$3,$C$4), "f, ", ROUND(F7/$C$3,$C$4), "f, ", ROUND(E7/$C$2,$C$4), "f);"))</f>
+        <v>title.Bounds = new Vector4(0.02853f, 0.04743f, 0.24901f, 0.94423f);</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -561,9 +574,9 @@
       <c r="F8" s="3">
         <v>40</v>
       </c>
-      <c r="G8" s="5" t="str">
-        <f t="shared" ref="G8:G31" si="0">CONCATENATE("new Vector4(", ROUND(C8/$C$2,$C$4), "f, ", ROUND(D8/$C$3,$C$4), "f, ", ROUND(F8/$C$3,$C$4), "f, ", ROUND(E8/$C$2,$C$4), "f)")</f>
-        <v>new Vector4(0.02853f, 0.32016f, 0.07905f, 0.2594f)</v>
+      <c r="G8" s="6" t="str">
+        <f>IF(COUNTBLANK(B8:F8)&gt;0,"",CONCATENATE(B8,".Bounds = new Vector4(", ROUND(C8/$C$2,$C$4), "f, ", ROUND(D8/$C$3,$C$4), "f, ", ROUND(F8/$C$3,$C$4), "f, ", ROUND(E8/$C$2,$C$4), "f);"))</f>
+        <v>new.Bounds = new Vector4(0.02853f, 0.32016f, 0.07905f, 0.2594f);</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -582,9 +595,9 @@
       <c r="F9" s="3">
         <v>40</v>
       </c>
-      <c r="G9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0.06226f, 0.42688f, 0.07905f, 0.2594f)</v>
+      <c r="G9" s="6" t="str">
+        <f t="shared" ref="G9:G30" si="0">IF(COUNTBLANK(B9:F9)&gt;0,"",CONCATENATE(B9,".Bounds = new Vector4(", ROUND(C9/$C$2,$C$4), "f, ", ROUND(D9/$C$3,$C$4), "f, ", ROUND(F9/$C$3,$C$4), "f, ", ROUND(E9/$C$2,$C$4), "f);"))</f>
+        <v>load.Bounds = new Vector4(0.06226f, 0.42688f, 0.07905f, 0.2594f);</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -603,9 +616,9 @@
       <c r="F10" s="3">
         <v>40</v>
       </c>
-      <c r="G10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0.09598f, 0.53162f, 0.07905f, 0.2594f)</v>
+      <c r="G10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>settings.Bounds = new Vector4(0.09598f, 0.53162f, 0.07905f, 0.2594f);</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -624,9 +637,9 @@
       <c r="F11" s="3">
         <v>40</v>
       </c>
-      <c r="G11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0.131f, 0.63834f, 0.07905f, 0.2594f)</v>
+      <c r="G11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>exit.Bounds = new Vector4(0.131f, 0.63834f, 0.07905f, 0.2594f);</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -645,123 +658,128 @@
       <c r="F12" s="3">
         <v>323</v>
       </c>
-      <c r="G12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0.44099f, 0.32016f, 0.63834f, 0.53178f)</v>
+      <c r="G12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>news.Bounds = new Vector4(0.44099f, 0.32016f, 0.63834f, 0.53178f);</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
+      <c r="G13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
+      <c r="G14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
+      <c r="G15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
-      </c>
-    </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Vector4(0f, 0f, 0f, 0f)</v>
+      <c r="G16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="7" t="str">
+        <f>IF(COUNTBLANK(B31:F31)&gt;0,"",CONCATENATE(B31,".Bounds = new Vector4(", ROUND(C31/$C$2,$C$4), "f, ", ROUND(D31/$C$3,$C$4), "f, ", ROUND(F31/$C$3,$C$4), "f, ", ROUND(E31/$C$2,$C$4), "f);"))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>